<commit_message>
Added results for 10,000 and 50,000 sample size runs. Updated code to print end time to file as well as console.
</commit_message>
<xml_diff>
--- a/CMPSC_360/04_FT_Psuedo_Neural_Network/FinalTask/Runtime_Estimates.xlsx
+++ b/CMPSC_360/04_FT_Psuedo_Neural_Network/FinalTask/Runtime_Estimates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Y1_PSU_CMPSC_360\FinalTask\FinalTask\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PSU_Class_Projects\CMPSC_360\04_FT_Psuedo_Neural_Network\FinalTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -243,10 +243,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$5</c:f>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>100</c:v>
                 </c:pt>
@@ -258,16 +258,22 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$5</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -279,6 +285,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1360</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -286,7 +295,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-054A-430D-ACC5-E4C69AB895FB}"/>
+              <c16:uniqueId val="{00000002-4AFB-4004-890C-B6BBD48D01F2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -802,37 +811,37 @@
                   <c:v>18.245999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>161.64599999999999</c:v>
+                  <c:v>162.40930000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>649.04600000000005</c:v>
+                  <c:v>428.80930000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4947.5460000000003</c:v>
+                  <c:v>1479.8093000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16646.045999999998</c:v>
+                  <c:v>2780.8092999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39494.546000000002</c:v>
+                  <c:v>3956.8093000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77243.046000000002</c:v>
+                  <c:v>4632.8093000000008</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>133641.546</c:v>
+                  <c:v>4433.8092999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>212440.046</c:v>
+                  <c:v>2984.8093000000035</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>317388.54599999997</c:v>
+                  <c:v>-89.190700000000007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>452237.04599999997</c:v>
+                  <c:v>-5163.1907000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>620735.54599999997</c:v>
+                  <c:v>-12612.190699999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2620,10 +2629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,11 +2673,11 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <f>(5*10^(-9))*(A2^3)-(2*10^(-6))*(A2^2) +(0.0147)*(A2) + 0.546</f>
+        <f t="shared" ref="C2:C7" si="0">(5*10^(-9))*(A2^3)-(2*10^(-6))*(A2^2) +(0.0147)*(A2) + 0.546</f>
         <v>2.0010000000000003</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:E14" si="0">C2/60</f>
+        <f t="shared" ref="D2:E14" si="1">C2/60</f>
         <v>3.3350000000000005E-2</v>
       </c>
       <c r="E2">
@@ -2688,19 +2697,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <f>(5*10^(-9))*(A3^3)-(2*10^(-6))*(A3^2) +(0.0147)*(A3) + 0.546</f>
+        <f t="shared" si="0"/>
         <v>8.020999999999999</v>
       </c>
       <c r="D3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13368333333333332</v>
       </c>
       <c r="E3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.2280555555555552E-3</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F16" si="1">E3/24</f>
+        <f t="shared" ref="F3:F15" si="2">E3/24</f>
         <v>9.2835648148148137E-5</v>
       </c>
     </row>
@@ -2712,19 +2721,19 @@
         <v>18</v>
       </c>
       <c r="C4">
-        <f>(5*10^(-9))*(A4^3)-(2*10^(-6))*(A4^2) +(0.0147)*(A4) + 0.546</f>
+        <f t="shared" si="0"/>
         <v>18.245999999999999</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.30409999999999998</v>
       </c>
       <c r="E4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.0683333333333327E-3</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1118055555555552E-4</v>
       </c>
     </row>
@@ -2736,20 +2745,20 @@
         <v>153</v>
       </c>
       <c r="C5">
-        <f>(5*10^(-9))*(A5^3)-(2*10^(-6))*(A5^2) +(0.0147)*(A5) + 0.546</f>
-        <v>161.64599999999999</v>
+        <f>(-5*10^(-10))*(A5^3)+(2*10^(-5))*(A5^2)-(0.0023)*(A5) + 2.8093</f>
+        <v>162.40930000000003</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>2.6940999999999997</v>
+        <f t="shared" si="1"/>
+        <v>2.7068216666666673</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>4.4901666666666659E-2</v>
+        <f t="shared" si="1"/>
+        <v>4.5113694444444456E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
-        <v>1.8709027777777775E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.8797372685185191E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2757,41 +2766,44 @@
         <v>5000</v>
       </c>
       <c r="C6">
-        <f>(5*10^(-9))*(A6^3)-(2*10^(-6))*(A6^2) +(0.0147)*(A6) + 0.546</f>
-        <v>649.04600000000005</v>
+        <f t="shared" ref="C6:C15" si="3">(-5*10^(-10))*(A6^3)+(2*10^(-5))*(A6^2)-(0.0023)*(A6) + 2.8093</f>
+        <v>428.80930000000006</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>10.817433333333334</v>
+        <f t="shared" si="1"/>
+        <v>7.1468216666666677</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0.18029055555555557</v>
+        <f t="shared" si="1"/>
+        <v>0.11911369444444446</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>7.5121064814814816E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.9630706018518522E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10000</v>
       </c>
+      <c r="B7">
+        <v>1360</v>
+      </c>
       <c r="C7">
-        <f>(5*10^(-9))*(A7^3)-(2*10^(-6))*(A7^2) +(0.0147)*(A7) + 0.546</f>
-        <v>4947.5460000000003</v>
+        <f t="shared" si="3"/>
+        <v>1479.8093000000001</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>82.459100000000007</v>
+        <f t="shared" si="1"/>
+        <v>24.663488333333337</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>1.3743183333333335</v>
+        <f t="shared" si="1"/>
+        <v>0.41105813888888892</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>5.7263263888888895E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.7127422453703706E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2799,20 +2811,20 @@
         <v>15000</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C16" si="2">(5*10^(-9))*(A8^3)-(2*10^(-6))*(A8^2) +(0.0147)*(A8) + 0.546</f>
-        <v>16646.045999999998</v>
+        <f t="shared" si="3"/>
+        <v>2780.8092999999999</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>277.4341</v>
+        <f t="shared" si="1"/>
+        <v>46.346821666666663</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>4.6239016666666668</v>
+        <f t="shared" si="1"/>
+        <v>0.77244702777777774</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>0.19266256944444446</v>
+        <f t="shared" si="2"/>
+        <v>3.218529282407407E-2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2820,20 +2832,20 @@
         <v>20000</v>
       </c>
       <c r="C9">
+        <f t="shared" si="3"/>
+        <v>3956.8093000000003</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>65.946821666666679</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.0991136944444446</v>
+      </c>
+      <c r="F9">
         <f t="shared" si="2"/>
-        <v>39494.546000000002</v>
-      </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>658.24243333333334</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>10.970707222222222</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>0.45711280092592593</v>
+        <v>4.5796403935185193E-2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2841,20 +2853,20 @@
         <v>25000</v>
       </c>
       <c r="C10">
+        <f t="shared" si="3"/>
+        <v>4632.8093000000008</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>77.213488333333345</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1.2868914722222224</v>
+      </c>
+      <c r="F10">
         <f t="shared" si="2"/>
-        <v>77243.046000000002</v>
-      </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>1287.3841</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>21.456401666666668</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>0.89401673611111121</v>
+        <v>5.3620478009259266E-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2862,20 +2874,20 @@
         <v>30000</v>
       </c>
       <c r="C11">
+        <f t="shared" si="3"/>
+        <v>4433.8092999999999</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>73.896821666666668</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>1.2316136944444445</v>
+      </c>
+      <c r="F11">
         <f t="shared" si="2"/>
-        <v>133641.546</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>2227.3591000000001</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>37.12265166666667</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>1.5467771527777778</v>
+        <v>5.1317237268518522E-2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2883,20 +2895,20 @@
         <v>35000</v>
       </c>
       <c r="C12">
+        <f t="shared" si="3"/>
+        <v>2984.8093000000035</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>49.746821666666726</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.82911369444444538</v>
+      </c>
+      <c r="F12">
         <f t="shared" si="2"/>
-        <v>212440.046</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>3540.6674333333335</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>59.011123888888889</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>2.4587968287037039</v>
+        <v>3.4546403935185224E-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2904,20 +2916,20 @@
         <v>40000</v>
       </c>
       <c r="C13">
+        <f t="shared" si="3"/>
+        <v>-89.190700000000007</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>-1.4865116666666667</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>-2.4775194444444443E-2</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="2"/>
-        <v>317388.54599999997</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>5289.8090999999995</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="0"/>
-        <v>88.163484999999994</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>3.6734785416666664</v>
+        <v>-1.0322997685185185E-3</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2925,20 +2937,20 @@
         <v>45000</v>
       </c>
       <c r="C14">
+        <f t="shared" si="3"/>
+        <v>-5163.1907000000001</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>-86.053178333333335</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>-1.4342196388888888</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="2"/>
-        <v>452237.04599999997</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>7537.2840999999999</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="0"/>
-        <v>125.62140166666667</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>5.2342250694444443</v>
+        <v>-5.975915162037037E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,20 +2958,85 @@
         <v>50000</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
-        <v>620735.54599999997</v>
+        <f t="shared" si="3"/>
+        <v>-12612.190699999999</v>
       </c>
       <c r="D15">
         <f>C15/60</f>
-        <v>10345.592433333333</v>
+        <v>-210.20317833333331</v>
       </c>
       <c r="E15">
-        <f t="shared" ref="E15:E16" si="3">D15/60</f>
-        <v>172.42654055555556</v>
+        <f t="shared" ref="E15" si="4">D15/60</f>
+        <v>-3.5033863055555554</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>7.1844391898148148</v>
+        <f t="shared" si="2"/>
+        <v>-0.14597442939814814</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <f>A22/B22</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>500</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ref="C23:C27" si="5">A23/B23</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1000</v>
+      </c>
+      <c r="B24">
+        <v>18</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="5"/>
+        <v>55.555555555555557</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3000</v>
+      </c>
+      <c r="B25">
+        <v>153</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="5"/>
+        <v>19.607843137254903</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10000</v>
+      </c>
+      <c r="B27">
+        <v>1360</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="5"/>
+        <v>7.3529411764705879</v>
       </c>
     </row>
   </sheetData>

</xml_diff>